<commit_message>
Added a first-pass on more rooms and enemies.
Added a first-pass on a forest region and populated the world with enemies from levels 1 to 5. A few minor tweaks and bug fixes as well.
</commit_message>
<xml_diff>
--- a/Borealis/Borealis Map.xlsx
+++ b/Borealis/Borealis Map.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Aurora\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Aurora\Borealis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1D202B0-6A83-450B-9BC0-B408DBD4FB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F616C9-16CF-4779-B546-36B04B4E0004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BFFA35C8-D8ED-45F3-84EB-2F18BCD67EE4}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{BFFA35C8-D8ED-45F3-84EB-2F18BCD67EE4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Map" sheetId="1" r:id="rId1"/>
+    <sheet name="Enemies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>0 - Limbo</t>
   </si>
@@ -82,6 +83,162 @@
   </si>
   <si>
     <t>15 - Road Out of Town</t>
+  </si>
+  <si>
+    <t>16 - Cathedral Basement</t>
+  </si>
+  <si>
+    <t>up/down</t>
+  </si>
+  <si>
+    <t>17 - Cobbled Path</t>
+  </si>
+  <si>
+    <t>18 - Stone Bridge</t>
+  </si>
+  <si>
+    <t>19 - River Crossing</t>
+  </si>
+  <si>
+    <t>20 - Rambling Creek</t>
+  </si>
+  <si>
+    <t>21 - Rocky Coast</t>
+  </si>
+  <si>
+    <t>22 - Forest Entrance</t>
+  </si>
+  <si>
+    <t>25 - Grassy Hill</t>
+  </si>
+  <si>
+    <t>24 - Wooded Grove</t>
+  </si>
+  <si>
+    <t>23 - Shaded Hollow</t>
+  </si>
+  <si>
+    <t>deranged seagull (lvl 1)</t>
+  </si>
+  <si>
+    <t>rabid rat (lvl 1)</t>
+  </si>
+  <si>
+    <t>remorhaz (lvl 2)</t>
+  </si>
+  <si>
+    <t>brown bear (lvl 3)</t>
+  </si>
+  <si>
+    <t>wild boar (lvl 2)</t>
+  </si>
+  <si>
+    <t>grey wolf (lvl 3)</t>
+  </si>
+  <si>
+    <t>hungry lynx (lvl 2)</t>
+  </si>
+  <si>
+    <t>giant troll (lvl 5)</t>
+  </si>
+  <si>
+    <t>ferocious wolverine (lvl 4)</t>
+  </si>
+  <si>
+    <t>venomous snake (lvl 1)</t>
+  </si>
+  <si>
+    <t>polar bear (lvl 4)</t>
+  </si>
+  <si>
+    <t>decaying draugr (lvl 5)</t>
+  </si>
+  <si>
+    <t>26 - Cave Entrance</t>
+  </si>
+  <si>
+    <t>27 - Dark Brambles</t>
+  </si>
+  <si>
+    <t>28  - Cave Interior</t>
+  </si>
+  <si>
+    <t>29 - Cavernous Opening</t>
+  </si>
+  <si>
+    <t>30 - Dank Dead End</t>
+  </si>
+  <si>
+    <t>31 - Narrow Tunnel</t>
+  </si>
+  <si>
+    <t>32 - The Den</t>
+  </si>
+  <si>
+    <t>rabid rat</t>
+  </si>
+  <si>
+    <t>deranged seagull</t>
+  </si>
+  <si>
+    <t>venomous snake</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>base stats</t>
+  </si>
+  <si>
+    <t>level multiplier</t>
+  </si>
+  <si>
+    <t>Max HP</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>XP</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>remorhaz</t>
+  </si>
+  <si>
+    <t>hungry lynx</t>
+  </si>
+  <si>
+    <t>wild boar</t>
+  </si>
+  <si>
+    <t>brown bear</t>
+  </si>
+  <si>
+    <t>grey wolf</t>
+  </si>
+  <si>
+    <t>ferocious wolverine</t>
+  </si>
+  <si>
+    <t>polar bear</t>
+  </si>
+  <si>
+    <t>decaying draugr</t>
+  </si>
+  <si>
+    <t>giant troll</t>
   </si>
 </sst>
 </file>
@@ -207,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -217,6 +374,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,26 +695,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B725E0-BE02-4D07-80A2-44DD3FFFFCFD}">
-  <dimension ref="B1:O21"/>
+  <dimension ref="B1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W21" sqref="W21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.578125" customWidth="1"/>
+    <col min="1" max="1" width="3.578125" customWidth="1"/>
     <col min="2" max="3" width="10.578125" customWidth="1"/>
-    <col min="4" max="4" width="5.578125" customWidth="1"/>
+    <col min="4" max="4" width="3.578125" customWidth="1"/>
     <col min="5" max="6" width="10.578125" customWidth="1"/>
-    <col min="7" max="7" width="5.578125" customWidth="1"/>
+    <col min="7" max="7" width="3.578125" customWidth="1"/>
     <col min="8" max="9" width="10.578125" customWidth="1"/>
-    <col min="10" max="10" width="5.578125" customWidth="1"/>
+    <col min="10" max="10" width="3.578125" customWidth="1"/>
     <col min="11" max="12" width="10.578125" customWidth="1"/>
-    <col min="13" max="13" width="5.578125" customWidth="1"/>
+    <col min="13" max="13" width="3.578125" customWidth="1"/>
     <col min="14" max="15" width="10.578125" customWidth="1"/>
+    <col min="16" max="16" width="3.578125" customWidth="1"/>
+    <col min="17" max="18" width="10.578125" customWidth="1"/>
+    <col min="19" max="19" width="3.578125" customWidth="1"/>
+    <col min="20" max="21" width="10.578125" customWidth="1"/>
+    <col min="22" max="22" width="3.578125" customWidth="1"/>
+    <col min="23" max="24" width="10.578125" customWidth="1"/>
+    <col min="25" max="25" width="3.578125" customWidth="1"/>
+    <col min="26" max="27" width="10.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
@@ -570,9 +744,15 @@
         <v>14</v>
       </c>
       <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B3" s="4"/>
+      <c r="T2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="3"/>
+    </row>
+    <row r="3" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
@@ -580,14 +760,19 @@
       <c r="I3" s="5"/>
       <c r="K3" s="4"/>
       <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="8"/>
       <c r="E4" s="7"/>
       <c r="H4" s="8"/>
       <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -598,22 +783,29 @@
       </c>
       <c r="I5" s="3"/>
       <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="E6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
       <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T6" s="4"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B7" s="7"/>
       <c r="E7" s="7"/>
       <c r="H7" s="7"/>
       <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -638,8 +830,18 @@
         <v>15</v>
       </c>
       <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="E9" s="4"/>
@@ -650,12 +852,19 @@
       <c r="L9" s="5"/>
       <c r="N9" s="4"/>
       <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q9" s="4"/>
+      <c r="R9" s="5"/>
+      <c r="T9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E10" s="7"/>
       <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.55000000000000004">
       <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
@@ -664,47 +873,684 @@
         <v>12</v>
       </c>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T12" s="4"/>
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="T13" s="7"/>
+    </row>
+    <row r="14" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R14" s="3"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" s="3"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X14" s="3"/>
+    </row>
+    <row r="15" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="2" t="s">
+      <c r="Q15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="5"/>
+      <c r="T15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U15" s="5"/>
+      <c r="W15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X15" s="5"/>
+    </row>
+    <row r="16" spans="2:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="T16" s="7"/>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="T17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U17" s="3"/>
+      <c r="W17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17" s="3"/>
+    </row>
+    <row r="18" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="5"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="5"/>
+    </row>
+    <row r="19" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T19" s="7"/>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U20" s="3"/>
+      <c r="W20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X20" s="3"/>
+    </row>
+    <row r="21" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
+      <c r="T21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U21" s="5"/>
+      <c r="W21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="X21" s="5"/>
+    </row>
+    <row r="22" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="W23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA23" s="3"/>
+    </row>
+    <row r="24" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="W24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="X24" s="5"/>
+      <c r="Z24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA24" s="5"/>
+    </row>
+    <row r="25" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="W25" s="7"/>
+    </row>
+    <row r="26" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U26" s="3"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X26" s="3"/>
+    </row>
+    <row r="27" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="T27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U27" s="5"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E16:F16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9CE05F-309B-4C47-B4B9-BC089EA5DA51}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="16.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>10</v>
+      </c>
+      <c r="I1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="10">
+        <f>(D$1+D$2*($B5-1))*$C5</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" ref="E5:I16" si="0">(E$1+E$2*($B5-1))*$C5</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" ref="D6:D16" si="1">(D$1+D$2*($B6-1))*$C6</f>
+        <v>10</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.2</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>11.200000000000001</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="0"/>
+        <v>22.400000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10">
+        <f>(D$1+D$2*($B9-1))*$C9</f>
+        <v>15</v>
+      </c>
+      <c r="E9" s="10">
+        <f>(E$1+E$2*($B9-1))*$C9</f>
+        <v>6</v>
+      </c>
+      <c r="F9" s="10">
+        <f>(F$1+F$2*($B9-1))*$C9</f>
+        <v>6</v>
+      </c>
+      <c r="G9" s="10">
+        <f>(G$1+G$2*($B9-1))*$C9</f>
+        <v>6</v>
+      </c>
+      <c r="H9" s="10">
+        <f>(H$1+H$2*($B9-1))*$C9</f>
+        <v>14</v>
+      </c>
+      <c r="I9" s="10">
+        <f>(I$1+I$2*($B9-1))*$C9</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="0"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="0"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="0"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="0"/>
+        <v>16.8</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="0"/>
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G11" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>1.2</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="0"/>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="0"/>
+        <v>43.199999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="10">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>1.2</v>
+      </c>
+      <c r="D14" s="10">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="0"/>
+        <v>9.6</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="0"/>
+        <v>9.6</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>9.6</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="0"/>
+        <v>26.4</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="0"/>
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1.2</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="0"/>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="0"/>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="0"/>
+        <v>31.2</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="0"/>
+        <v>62.4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>